<commit_message>
make SRD from PD
</commit_message>
<xml_diff>
--- a/05_2nd Subimittal/zone_list_2nd.xlsx
+++ b/05_2nd Subimittal/zone_list_2nd.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyunwoo\github\1300_NE_45th\05_AfterSubmittal_change\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyunwoo\github\1300_NE_45th\05_2nd Subimittal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1587E719-DFEB-4597-B20A-6C2F9B003B33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C818D0C-CA65-46C1-9880-C7D507B4B914}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6045" yWindow="3105" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="zone_list_2nd" sheetId="2" r:id="rId1"/>
-    <sheet name="zone_list" sheetId="1" r:id="rId2"/>
+    <sheet name="zone_list_1st" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">zone_list!$A$1:$J$183</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">zone_list_1st!$A$1:$J$183</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">zone_list_2nd!$A$1:$J$183</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -34,8 +34,35 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={92041B2F-F118-4EEA-8D3E-DBD23CEB3235}</author>
+    <author>tc={8D8D110C-240D-403F-B2C3-C2E2C4AECE0C}</author>
+  </authors>
+  <commentList>
+    <comment ref="I12" authorId="0" shapeId="0" xr:uid="{92041B2F-F118-4EEA-8D3E-DBD23CEB3235}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    VRF?</t>
+      </text>
+    </comment>
+    <comment ref="I48" authorId="1" shapeId="0" xr:uid="{8D8D110C-240D-403F-B2C3-C2E2C4AECE0C}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    VRF?</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1848" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1857" uniqueCount="437">
   <si>
     <t>Zone Names</t>
   </si>
@@ -1340,13 +1367,19 @@
   </si>
   <si>
     <t>THERMAL ZONE: STOR_0101C</t>
+  </si>
+  <si>
+    <t>SplitHP-OFFICE</t>
+  </si>
+  <si>
+    <t>SplitHP-LAUN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1464,8 +1497,14 @@
       <name val="Calibri Light"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1645,6 +1684,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1806,9 +1851,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1865,6 +1912,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Hyunwoo Lim" id="{356ED1F7-C36A-4D02-A819-99FCB6035B41}" userId="de2010b060398c3e" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2162,12 +2215,23 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="I12" dT="2020-12-01T22:54:51.00" personId="{356ED1F7-C36A-4D02-A819-99FCB6035B41}" id="{92041B2F-F118-4EEA-8D3E-DBD23CEB3235}">
+    <text>VRF?</text>
+  </threadedComment>
+  <threadedComment ref="I48" dT="2020-12-01T22:54:51.00" personId="{356ED1F7-C36A-4D02-A819-99FCB6035B41}" id="{8D8D110C-240D-403F-B2C3-C2E2C4AECE0C}">
+    <text>VRF?</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0665169F-D150-4A58-B4BE-D75D65FBC2ED}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0665169F-D150-4A58-B4BE-D75D65FBC2ED}">
   <dimension ref="A1:N185"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2262,7 +2326,7 @@
         <v>431</v>
       </c>
       <c r="F3">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="G3" t="s">
         <v>418</v>
@@ -2292,7 +2356,7 @@
         <v>431</v>
       </c>
       <c r="F4">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="G4" t="s">
         <v>418</v>
@@ -2322,7 +2386,7 @@
         <v>431</v>
       </c>
       <c r="F5">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="G5" t="s">
         <v>418</v>
@@ -2334,199 +2398,211 @@
         <v>395</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="B6" t="str">
+      <c r="B6" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> AMEN_2204</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D6" t="s">
-        <v>388</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="D6" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="2">
         <v>1200</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="J6" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="J6" s="2" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="B7" t="str">
+      <c r="B7" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> AMEN_2205</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D7" t="s">
-        <v>388</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="D7" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
         <v>40</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="2" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="B8" t="str">
+      <c r="B8" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> AMEN_FITNESS_2202</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D8" t="s">
-        <v>388</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="D8" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2">
         <v>35</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="2" t="s">
         <v>414</v>
       </c>
       <c r="J8" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="B9" t="str">
+      <c r="B9" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> AMEN_SKYLOUNGE_2201</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D9" t="s">
-        <v>388</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="D9" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="2">
         <v>145</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="2" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="B10" t="str">
+      <c r="B10" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> AMEN_STORAGE_2204</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D10" t="s">
-        <v>388</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="D10" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="2">
         <v>400</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="2" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="B11" t="str">
+      <c r="B11" s="2" t="str">
         <f>RIGHT(A11,LEN(A11)-FIND(": ",A11))</f>
         <v xml:space="preserve"> AMEN_SUNROOM_2203</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="D11" t="s">
-        <v>388</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="D11" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="G11" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B12" t="str">
+      <c r="B12" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> CORR_0100</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D12" t="s">
-        <v>388</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="D12" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="F12">
-        <v>95</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="F12" s="2">
+        <v>25</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="I12" t="s">
-        <v>392</v>
+      <c r="I12" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -2556,8 +2632,8 @@
         <v>392</v>
       </c>
       <c r="N13">
-        <f>SUM(F12:F46)</f>
-        <v>1250</v>
+        <f>SUM(F13:F19)</f>
+        <v>675</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -2833,57 +2909,57 @@
         <v>392</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="25" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="B25" t="str">
+      <c r="B25" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> ELEV LOBBY_P100</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D25" t="s">
-        <v>388</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="D25" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="F25">
-        <v>225</v>
-      </c>
-      <c r="G25" t="s">
+      <c r="F25" s="2">
+        <v>205</v>
+      </c>
+      <c r="G25" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I25" s="2" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="26" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B26" t="str">
+      <c r="B26" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> ELEV LOBBY_P200</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D26" t="s">
-        <v>388</v>
-      </c>
-      <c r="E26" t="s">
+      <c r="D26" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="F26">
-        <v>225</v>
-      </c>
-      <c r="G26" t="s">
+      <c r="F26" s="2">
+        <v>205</v>
+      </c>
+      <c r="G26" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I26" s="2" t="s">
         <v>392</v>
       </c>
     </row>
@@ -3187,112 +3263,121 @@
         <v>389</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="47" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B47" t="str">
+      <c r="B47" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> FCC_0100</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D47" t="s">
-        <v>388</v>
-      </c>
-      <c r="E47" t="s">
+      <c r="D47" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="2">
         <v>50</v>
       </c>
-      <c r="G47" t="s">
+      <c r="G47" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="I47" t="s">
+      <c r="I47" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="J47" t="s">
+      <c r="J47" s="2" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="48" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="B48" t="str">
+      <c r="B48" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> LAUNDRY_0109</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D48" t="s">
-        <v>388</v>
-      </c>
-      <c r="E48" t="s">
+      <c r="D48" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="E48" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="F48">
+      <c r="F48" s="2">
         <v>300</v>
       </c>
-      <c r="G48" t="s">
+      <c r="G48" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="I48" t="s">
-        <v>415</v>
-      </c>
-      <c r="J48" t="s">
+      <c r="I48" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="J48" s="2" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="49" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="B49" t="str">
+      <c r="B49" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> LOBBY_0101</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D49" t="s">
-        <v>388</v>
-      </c>
-      <c r="E49" t="s">
+      <c r="D49" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="E49" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="F49">
+      <c r="F49" s="2">
         <v>250</v>
       </c>
-      <c r="G49" t="s">
+      <c r="G49" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="I49" t="s">
+      <c r="I49" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="J49" t="s">
+      <c r="J49" s="2" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="50" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="B50" t="str">
+      <c r="B50" s="2" t="str">
         <f>RIGHT(A50,LEN(A50)-FIND(": ",A50))</f>
         <v xml:space="preserve"> MAIL_0101</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D50" t="s">
-        <v>388</v>
-      </c>
-      <c r="E50" t="s">
+      <c r="D50" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="E50" s="2" t="s">
         <v>431</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
@@ -3370,51 +3455,60 @@
         <v>389</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="56" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="B56" t="str">
+      <c r="B56" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> OFFICE_0101</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="D56" t="s">
-        <v>388</v>
-      </c>
-      <c r="E56" t="s">
+      <c r="D56" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="E56" s="2" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="F56" s="2">
+        <v>115</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="J56" s="2" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B57" t="str">
+      <c r="B57" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> PACKAGE_0100</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D57" t="s">
-        <v>388</v>
-      </c>
-      <c r="E57" t="s">
+      <c r="D57" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="E57" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="F57">
+      <c r="F57" s="2">
         <v>20</v>
       </c>
-      <c r="G57" t="s">
+      <c r="G57" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="I57" t="s">
-        <v>415</v>
-      </c>
-      <c r="J57" t="s">
+      <c r="J57" s="2" t="s">
         <v>393</v>
       </c>
     </row>
@@ -3472,30 +3566,30 @@
         <v>50</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="61" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B61" t="str">
+      <c r="B61" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> RETAIL_0100</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D61" t="s">
-        <v>388</v>
-      </c>
-      <c r="E61" t="s">
+      <c r="D61" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="E61" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="F61">
-        <v>505</v>
-      </c>
-      <c r="G61" t="s">
+      <c r="F61" s="2">
+        <v>480</v>
+      </c>
+      <c r="G61" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="I61" t="s">
+      <c r="I61" s="2" t="s">
         <v>390</v>
       </c>
     </row>
@@ -6174,6 +6268,7 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6181,8 +6276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N183"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>